<commit_message>
Documentation and clock files for production testing
</commit_message>
<xml_diff>
--- a/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
+++ b/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-127_CM_V3\GitHub\Cornell_CM_Rev3_HW\ClockBuilderPRO\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA6C976-4006-4954-89D0-F535FF6F39DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C55AA36-1E00-4E47-86DE-5C3C74681958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Configurations" sheetId="1" r:id="rId1"/>
+    <sheet name="ClockDistribution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="164">
   <si>
     <t>Out 1</t>
   </si>
@@ -134,6 +135,401 @@
   </si>
   <si>
     <t>Green cells indicate the input sources</t>
+  </si>
+  <si>
+    <t>R0Av3X01</t>
+  </si>
+  <si>
+    <t>R0Bv3X01</t>
+  </si>
+  <si>
+    <t>Quad #</t>
+  </si>
+  <si>
+    <t>Quad Letter</t>
+  </si>
+  <si>
+    <t>Ref #</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>FPGA #1 Step #1 Source</t>
+  </si>
+  <si>
+    <t>FPGA #1 Step #1 Freq</t>
+  </si>
+  <si>
+    <t>FPGA #2 Step #1 Source</t>
+  </si>
+  <si>
+    <t>FPGA #2 Step #1 Freq</t>
+  </si>
+  <si>
+    <t>R0A-2</t>
+  </si>
+  <si>
+    <t>R0A-3</t>
+  </si>
+  <si>
+    <t>R1A-3</t>
+  </si>
+  <si>
+    <t>R0A-1</t>
+  </si>
+  <si>
+    <t>R0A-4</t>
+  </si>
+  <si>
+    <t>R1A-4</t>
+  </si>
+  <si>
+    <t>R0A-6</t>
+  </si>
+  <si>
+    <t>R0A-7</t>
+  </si>
+  <si>
+    <t>R0A-0</t>
+  </si>
+  <si>
+    <t>R0A-5</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>R1Av3X01</t>
+  </si>
+  <si>
+    <t>R1Bv3X01</t>
+  </si>
+  <si>
+    <t>R1Cv3X01</t>
+  </si>
+  <si>
+    <t>R1A-0A</t>
+  </si>
+  <si>
+    <t>R1A-0</t>
+  </si>
+  <si>
+    <t>R1B-4</t>
+  </si>
+  <si>
+    <t>R1A-5</t>
+  </si>
+  <si>
+    <t>R1A-6</t>
+  </si>
+  <si>
+    <t>R1A-7</t>
+  </si>
+  <si>
+    <t>R1A-8</t>
+  </si>
+  <si>
+    <t>R1B-0A</t>
+  </si>
+  <si>
+    <t>R1B-0</t>
+  </si>
+  <si>
+    <t>R1B-1</t>
+  </si>
+  <si>
+    <t>R1B-2</t>
+  </si>
+  <si>
+    <t>R1B-3</t>
+  </si>
+  <si>
+    <t>R1B-5</t>
+  </si>
+  <si>
+    <t>R1B-6</t>
+  </si>
+  <si>
+    <t>F1B-7</t>
+  </si>
+  <si>
+    <t>R1B-8</t>
+  </si>
+  <si>
+    <t>R1C-0A</t>
+  </si>
+  <si>
+    <t>R1C-0</t>
+  </si>
+  <si>
+    <t>R1C-1</t>
+  </si>
+  <si>
+    <t>R1C-2</t>
+  </si>
+  <si>
+    <t>R1C-3</t>
+  </si>
+  <si>
+    <t>R1C-4</t>
+  </si>
+  <si>
+    <t>R1C-5</t>
+  </si>
+  <si>
+    <t>R1C-6</t>
+  </si>
+  <si>
+    <t>R1C-9</t>
+  </si>
+  <si>
+    <t>R1C-7</t>
+  </si>
+  <si>
+    <t>R1C-8</t>
+  </si>
+  <si>
+    <t>R1C-9A</t>
+  </si>
+  <si>
+    <t>OSC</t>
+  </si>
+  <si>
+    <t>Logic Clock Pins</t>
+  </si>
+  <si>
+    <t>FPGA #1
+Step #1
+Source</t>
+  </si>
+  <si>
+    <t>BF27/BF28</t>
+  </si>
+  <si>
+    <t>LHC_CLK</t>
+  </si>
+  <si>
+    <t>BE26/BE27</t>
+  </si>
+  <si>
+    <t>F1_XTAL_200</t>
+  </si>
+  <si>
+    <t>AT17/AU16</t>
+  </si>
+  <si>
+    <t>P33/P34</t>
+  </si>
+  <si>
+    <t>N32/M32</t>
+  </si>
+  <si>
+    <t>R18/R17</t>
+  </si>
+  <si>
+    <t>N19/N18</t>
+  </si>
+  <si>
+    <t>R1B-9</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Logic Clock Name (schematic)</t>
+  </si>
+  <si>
+    <t>Logic Clock Name (constraint file)</t>
+  </si>
+  <si>
+    <t>lf_x12_r0_clk</t>
+  </si>
+  <si>
+    <t>lf_x4_r0_clk</t>
+  </si>
+  <si>
+    <t>rt_x12_r0_clk</t>
+  </si>
+  <si>
+    <t>rt_x4_r0_clk</t>
+  </si>
+  <si>
+    <t>tcds40_clk</t>
+  </si>
+  <si>
+    <t>lhc_clk</t>
+  </si>
+  <si>
+    <t>clk_200</t>
+  </si>
+  <si>
+    <t>in_spare[2]</t>
+  </si>
+  <si>
+    <t>C29/C30</t>
+  </si>
+  <si>
+    <t>out_spare[2]</t>
+  </si>
+  <si>
+    <t>BG26/BG27</t>
+  </si>
+  <si>
+    <t>lf_r0_ab</t>
+  </si>
+  <si>
+    <t>lf_r1_ab</t>
+  </si>
+  <si>
+    <t>lf_r0_ad</t>
+  </si>
+  <si>
+    <t>lf_r1_ad</t>
+  </si>
+  <si>
+    <t>lf_r1_af</t>
+  </si>
+  <si>
+    <t>lf_r0_r</t>
+  </si>
+  <si>
+    <t>lf_r1_r</t>
+  </si>
+  <si>
+    <t>lf_r0_u</t>
+  </si>
+  <si>
+    <t>lf_r1_u</t>
+  </si>
+  <si>
+    <t>lf_r0_w</t>
+  </si>
+  <si>
+    <t>lf_r1_w</t>
+  </si>
+  <si>
+    <t>lf_r0_y</t>
+  </si>
+  <si>
+    <t>lf_r1_y</t>
+  </si>
+  <si>
+    <t>lf_ro_af</t>
+  </si>
+  <si>
+    <t>rt_r0_n</t>
+  </si>
+  <si>
+    <t>rt_r1_n</t>
+  </si>
+  <si>
+    <t>rt_r0_b</t>
+  </si>
+  <si>
+    <t>rt_r1_b</t>
+  </si>
+  <si>
+    <t>rt_r0_e</t>
+  </si>
+  <si>
+    <t>rt_r1_e</t>
+  </si>
+  <si>
+    <t>rt_r0_g</t>
+  </si>
+  <si>
+    <t>rt_r1_g</t>
+  </si>
+  <si>
+    <t>rt_r0_p</t>
+  </si>
+  <si>
+    <t>rt_r1_p</t>
+  </si>
+  <si>
+    <t>rt_r0_i</t>
+  </si>
+  <si>
+    <t>rt_r0_l</t>
+  </si>
+  <si>
+    <t>rt_r1_l</t>
+  </si>
+  <si>
+    <t>Vivado Constraints Name</t>
+  </si>
+  <si>
+    <t>rt_r1_i</t>
+  </si>
+  <si>
+    <t>FnL_X12_R0_CLK</t>
+  </si>
+  <si>
+    <t>FnL_X4_R0_CLK</t>
+  </si>
+  <si>
+    <t>FnR_X12_R0_CLK</t>
+  </si>
+  <si>
+    <t>FnR_X4_R0_CLK</t>
+  </si>
+  <si>
+    <t>Fn_TCDS40_CLK</t>
+  </si>
+  <si>
+    <t>FnFmSPARE2</t>
+  </si>
+  <si>
+    <t>FPGA#2</t>
+  </si>
+  <si>
+    <t>FPGA#1</t>
   </si>
 </sst>
 </file>
@@ -255,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,13 +674,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -298,6 +691,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,7 +1015,7 @@
   <dimension ref="A1:S54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,395 +1127,308 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="9"/>
+      <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>48</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8" t="s">
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11" s="1">
         <v>322.265625</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="9"/>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>48</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="8" t="s">
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="Q13" s="1">
         <v>322.265625</v>
       </c>
-      <c r="R13" s="8" t="s">
+      <c r="R13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="S13" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="9"/>
+      <c r="S14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10">
-        <v>320.64</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="10">
-        <v>320.64</v>
-      </c>
-      <c r="H15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="I15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="J15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="K15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="L15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="M15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="N15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="O15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="P15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="S15" s="9">
+      <c r="D15" s="9">
+        <v>320.64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="9">
+        <v>320.64</v>
+      </c>
+      <c r="H15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="I15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="J15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="K15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="L15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="M15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="N15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="O15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="P15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S15" s="8">
         <v>320.64</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="9"/>
+      <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="9">
         <v>40.08</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="10">
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="9">
         <v>40.08</v>
       </c>
-      <c r="H17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="I17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="J17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="K17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="L17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="M17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="N17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="O17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="P17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>320.64</v>
-      </c>
-      <c r="R17" s="8">
+      <c r="H17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="I17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="J17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="K17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="L17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="M17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="N17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="O17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="P17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>320.64</v>
+      </c>
+      <c r="R17" s="1">
         <v>40.08</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S17" s="8">
         <v>40.08</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="9"/>
+      <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13">
-        <v>320.64</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="12">
+        <v>320.64</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="12" t="s">
+      <c r="F19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="I19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="J19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="K19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="L19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="M19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="N19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="O19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="P19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="Q19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="R19" s="12">
-        <v>320.64</v>
-      </c>
-      <c r="S19" s="14">
+      <c r="H19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="I19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="J19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="K19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="L19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="M19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="N19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="O19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="P19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="R19" s="11">
+        <v>320.64</v>
+      </c>
+      <c r="S19" s="13">
         <v>320.64</v>
       </c>
     </row>
@@ -1130,19 +1442,299 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S23" s="1"/>
+      <c r="A23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1">
+        <v>320</v>
+      </c>
+      <c r="J23" s="1">
+        <v>160</v>
+      </c>
+      <c r="K23" s="1">
+        <v>300</v>
+      </c>
+      <c r="L23" s="1">
+        <v>150</v>
+      </c>
+      <c r="M23" s="1">
+        <v>280</v>
+      </c>
+      <c r="N23" s="1">
+        <v>140</v>
+      </c>
+      <c r="O23" s="1">
+        <v>260</v>
+      </c>
+      <c r="P23" s="1">
+        <v>130</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>240</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S24" s="1"/>
+      <c r="A24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="9">
+        <v>48</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="1">
+        <v>310</v>
+      </c>
+      <c r="J24" s="1">
+        <v>155</v>
+      </c>
+      <c r="K24" s="1">
+        <v>290</v>
+      </c>
+      <c r="L24" s="1">
+        <v>145</v>
+      </c>
+      <c r="M24" s="1">
+        <v>270</v>
+      </c>
+      <c r="N24" s="1">
+        <v>135</v>
+      </c>
+      <c r="O24" s="1">
+        <v>250</v>
+      </c>
+      <c r="P24" s="1">
+        <v>125</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>230</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S25" s="1"/>
+      <c r="A25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9">
+        <v>48</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="1">
+        <v>60</v>
+      </c>
+      <c r="I25" s="1">
+        <v>40</v>
+      </c>
+      <c r="J25" s="1">
+        <v>100</v>
+      </c>
+      <c r="K25" s="1">
+        <v>120</v>
+      </c>
+      <c r="L25" s="1">
+        <v>312</v>
+      </c>
+      <c r="M25" s="1">
+        <v>168</v>
+      </c>
+      <c r="N25" s="1">
+        <v>336</v>
+      </c>
+      <c r="O25" s="1">
+        <v>156</v>
+      </c>
+      <c r="P25" s="1">
+        <v>272</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>136</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S25" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S26" s="1"/>
+      <c r="A26" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="9">
+        <v>48</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="1">
+        <v>176</v>
+      </c>
+      <c r="I26" s="1">
+        <v>220</v>
+      </c>
+      <c r="J26" s="1">
+        <v>110</v>
+      </c>
+      <c r="K26" s="1">
+        <v>132</v>
+      </c>
+      <c r="L26" s="1">
+        <v>296</v>
+      </c>
+      <c r="M26" s="1">
+        <v>163</v>
+      </c>
+      <c r="N26" s="1">
+        <v>326</v>
+      </c>
+      <c r="O26" s="1">
+        <v>148</v>
+      </c>
+      <c r="P26" s="1">
+        <v>268</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>132</v>
+      </c>
+      <c r="R26" s="1">
+        <v>55</v>
+      </c>
+      <c r="S26" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S27" s="1"/>
+      <c r="A27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="9">
+        <v>48</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="1">
+        <v>116</v>
+      </c>
+      <c r="I27" s="1">
+        <v>232</v>
+      </c>
+      <c r="J27" s="1">
+        <v>174</v>
+      </c>
+      <c r="K27" s="1">
+        <v>348</v>
+      </c>
+      <c r="L27" s="1">
+        <v>310</v>
+      </c>
+      <c r="M27" s="1">
+        <v>170</v>
+      </c>
+      <c r="N27" s="1">
+        <v>340</v>
+      </c>
+      <c r="O27" s="1">
+        <v>155</v>
+      </c>
+      <c r="P27" s="1">
+        <v>286</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>143</v>
+      </c>
+      <c r="R27" s="1">
+        <v>226</v>
+      </c>
+      <c r="S27" s="8">
+        <v>113</v>
+      </c>
     </row>
     <row r="35" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S35" s="1"/>
@@ -1199,4 +1791,995 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30567707-92ED-4587-9464-529A88E1A3E7}">
+  <dimension ref="A1:U32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="3.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="13" max="13" width="16.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="3.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="1">
+        <v>60</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1">
+        <v>40</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="1">
+        <v>300</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>120</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="1">
+        <v>220</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="1">
+        <v>110</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R6" s="1">
+        <v>150</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1">
+        <v>300</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="1">
+        <v>260</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="1">
+        <v>160</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U7" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>122</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1">
+        <v>132</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="1">
+        <v>148</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" s="1">
+        <v>280</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U8" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>124</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1">
+        <v>150</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="1">
+        <v>130</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R9" s="1">
+        <v>55</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U9" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="1">
+        <v>168</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="1">
+        <v>156</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R10" s="1">
+        <v>40</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="U10" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>126</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1">
+        <v>300</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="1">
+        <v>260</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="R11" s="1">
+        <v>200</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U11" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>126</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="1">
+        <v>296</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>129</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="1">
+        <v>300</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>129</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="1">
+        <v>176</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>131</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1">
+        <v>150</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>131</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="1">
+        <v>312</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="1">
+        <v>336</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>133</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1">
+        <v>300</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>133</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="1">
+        <v>163</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="1">
+        <v>134</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>220</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="1">
+        <v>200</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>220</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="1">
+        <v>272</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" s="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>222</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1">
+        <v>160</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>222</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="1">
+        <v>170</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>224</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="1">
+        <v>280</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>224</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="1">
+        <v>116</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>226</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="1">
+        <v>160</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>226</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="1">
+        <v>155</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>229</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="1">
+        <v>160</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>229</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="1">
+        <v>286</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>231</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="1">
+        <v>280</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J29" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>231</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="1">
+        <v>143</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>233</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="1">
+        <v>160</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>233</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="1">
+        <v>113</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="1">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added synth config files for testing R0A and R0B inputs
</commit_message>
<xml_diff>
--- a/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
+++ b/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-127_CM_V3\GitHub\Cornell_CM_Rev3_HW\ClockBuilderPRO\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0356376C-E15A-4AF2-A6A7-942E8B51B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58160371-3CCC-40EE-99BD-87A05E8DFF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
   </bookViews>
   <sheets>
     <sheet name="Configurations" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="199">
   <si>
     <t>Out 1</t>
   </si>
@@ -623,6 +623,18 @@
   </si>
   <si>
     <t>F2R_X4_R0_SEL</t>
+  </si>
+  <si>
+    <t>R0Bv3X02</t>
+  </si>
+  <si>
+    <t>R0Bv3X03</t>
+  </si>
+  <si>
+    <t>R0Bv3X04</t>
+  </si>
+  <si>
+    <t>R0Av3X02</t>
   </si>
 </sst>
 </file>
@@ -751,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -814,15 +826,22 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAA10E1-D638-4109-9638-B5E913BD74DD}">
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,10 +1582,28 @@
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+    </row>
+    <row r="23" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>33</v>
       </c>
@@ -1625,276 +1662,587 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="26">
+        <v>230</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="26">
+        <v>230</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="25">
+        <v>230</v>
+      </c>
+      <c r="J24" s="25">
+        <v>230</v>
+      </c>
+      <c r="K24" s="25">
+        <v>230</v>
+      </c>
+      <c r="L24" s="25">
+        <v>230</v>
+      </c>
+      <c r="M24" s="25">
+        <v>230</v>
+      </c>
+      <c r="N24" s="25">
+        <v>230</v>
+      </c>
+      <c r="O24" s="25">
+        <v>230</v>
+      </c>
+      <c r="P24" s="25">
+        <v>230</v>
+      </c>
+      <c r="Q24" s="25">
+        <v>230</v>
+      </c>
+      <c r="R24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" s="8">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B26" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C26" s="26">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="D26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I26" s="25">
         <v>310</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J26" s="25">
         <v>155</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K26" s="25">
         <v>290</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L26" s="25">
         <v>145</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M26" s="25">
         <v>270</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N26" s="25">
         <v>135</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O26" s="25">
         <v>250</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P26" s="25">
         <v>125</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="Q26" s="25">
         <v>230</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="R26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="S24" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="S26" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26">
+        <v>240</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="26">
+        <v>240</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="25">
+        <v>240</v>
+      </c>
+      <c r="J27" s="25">
+        <v>240</v>
+      </c>
+      <c r="K27" s="25">
+        <v>240</v>
+      </c>
+      <c r="L27" s="25">
+        <v>240</v>
+      </c>
+      <c r="M27" s="25">
+        <v>240</v>
+      </c>
+      <c r="N27" s="25">
+        <v>240</v>
+      </c>
+      <c r="O27" s="25">
+        <v>240</v>
+      </c>
+      <c r="P27" s="25">
+        <v>240</v>
+      </c>
+      <c r="Q27" s="25">
+        <v>240</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="S27" s="8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="26">
+        <v>320</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="26">
+        <v>320</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="25">
+        <v>320</v>
+      </c>
+      <c r="J28" s="25">
+        <v>320</v>
+      </c>
+      <c r="K28" s="25">
+        <v>320</v>
+      </c>
+      <c r="L28" s="25">
+        <v>320</v>
+      </c>
+      <c r="M28" s="25">
+        <v>320</v>
+      </c>
+      <c r="N28" s="25">
+        <v>320</v>
+      </c>
+      <c r="O28" s="25">
+        <v>320</v>
+      </c>
+      <c r="P28" s="25">
+        <v>320</v>
+      </c>
+      <c r="Q28" s="25">
+        <v>320</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="S28" s="8">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="26">
+        <v>40</v>
+      </c>
+      <c r="G29" s="26">
+        <v>40</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="25">
+        <v>200</v>
+      </c>
+      <c r="J29" s="25">
+        <v>200</v>
+      </c>
+      <c r="K29" s="25">
+        <v>200</v>
+      </c>
+      <c r="L29" s="25">
+        <v>200</v>
+      </c>
+      <c r="M29" s="25">
+        <v>200</v>
+      </c>
+      <c r="N29" s="25">
+        <v>200</v>
+      </c>
+      <c r="O29" s="25">
+        <v>200</v>
+      </c>
+      <c r="P29" s="25">
+        <v>200</v>
+      </c>
+      <c r="Q29" s="25">
+        <v>200</v>
+      </c>
+      <c r="R29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="S29" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B31" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C31" s="26">
         <v>48</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="D31" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="25">
         <v>60</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I31" s="25">
         <v>40</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J31" s="25">
         <v>100</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K31" s="25">
         <v>120</v>
       </c>
-      <c r="L25" s="1">
+      <c r="L31" s="25">
         <v>312</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M31" s="25">
         <v>168</v>
       </c>
-      <c r="N25" s="1">
+      <c r="N31" s="25">
         <v>336</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O31" s="25">
         <v>156</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P31" s="25">
         <v>272</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="Q31" s="25">
         <v>136</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="R31" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="S25" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="S31" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B33" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C33" s="26">
         <v>48</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="D33" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="25">
         <v>176</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I33" s="25">
         <v>220</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J33" s="25">
         <v>110</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K33" s="25">
         <v>132</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L33" s="25">
         <v>296</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M33" s="25">
         <v>163</v>
       </c>
-      <c r="N26" s="1">
+      <c r="N33" s="25">
         <v>326</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O33" s="25">
         <v>148</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P33" s="25">
         <v>268</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q33" s="25">
         <v>132</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R33" s="25">
         <v>55</v>
       </c>
-      <c r="S26" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="S33" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C35" s="12">
         <v>48</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="D35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="11" t="s">
+      <c r="F35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H35" s="11">
         <v>116</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I35" s="11">
         <v>232</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J35" s="11">
         <v>174</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K35" s="11">
         <v>348</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L35" s="11">
         <v>310</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M35" s="11">
         <v>170</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N35" s="11">
         <v>340</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O35" s="11">
         <v>155</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P35" s="11">
         <v>286</v>
       </c>
-      <c r="Q27" s="11">
+      <c r="Q35" s="11">
         <v>143</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R35" s="11">
         <v>226</v>
       </c>
-      <c r="S27" s="13">
+      <c r="S35" s="13">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S37" s="1"/>
-    </row>
-    <row r="39" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S39" s="1"/>
-    </row>
-    <row r="40" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S41" s="1"/>
-    </row>
-    <row r="42" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S42" s="1"/>
-    </row>
-    <row r="43" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S43" s="1"/>
     </row>
-    <row r="45" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S46" s="1"/>
-    </row>
-    <row r="47" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.25">
@@ -1903,14 +2251,35 @@
     <row r="50" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S50" s="1"/>
     </row>
-    <row r="52" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S52" s="1"/>
+    <row r="51" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S51" s="1"/>
     </row>
     <row r="53" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S53" s="1"/>
     </row>
     <row r="54" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S54" s="1"/>
+    </row>
+    <row r="55" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S55" s="1"/>
+    </row>
+    <row r="56" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S58" s="1"/>
+    </row>
+    <row r="60" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1922,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30567707-92ED-4587-9464-529A88E1A3E7}">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AE11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>